<commit_message>
training sql - bài tập day 2
</commit_message>
<xml_diff>
--- a/SQL-TRAINING.xlsx
+++ b/SQL-TRAINING.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damcong\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damcong\Desktop\training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A2A8C2E-2018-4587-8E6E-2A014A3F647F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43DA2EA-7180-4219-AE80-05BF4BB0101D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A73E0EEF-360B-49A0-9CAE-CE731E000F07}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A73E0EEF-360B-49A0-9CAE-CE731E000F07}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DAY 1" sheetId="1" r:id="rId1"/>
+    <sheet name="DAY 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>STT</t>
   </si>
@@ -91,14 +92,58 @@
 INNER JOIN Products ON Products.ProductID = OrderDetails.ProductID</t>
   </si>
   <si>
-    <t>BÀI TẬP SQL</t>
+    <t>CÂU TRUY VẤN</t>
+  </si>
+  <si>
+    <t>Tạo 1 view trong sql server ( gọi ra nhiều trường(&gt; 2))</t>
+  </si>
+  <si>
+    <t>Tạo 1 table function trong sql server (tra ra view vừa tạo)</t>
+  </si>
+  <si>
+    <t>Tạo 1 store proseduce có gọi table function trong sql server</t>
+  </si>
+  <si>
+    <t>CREATE VIEW NHANVIEN_VIEW AS
+SELECT ten, tuoi
+FROM NHANVIEN
+SELECT * FROM NHANVIEN_VIEW</t>
+  </si>
+  <si>
+    <t>CREATE FUNCTION func_nhanvien
+(
+@ten NVARCHAR(100),
+)
+RETURNS TABLE
+AS 
+RETURN 
+SELECT * FROM NHANVIEN_VIEW
+WHERE ten=@ten
+GO
+SELECT * FROM func_nhanvien('hiendam')</t>
+  </si>
+  <si>
+    <t>CREATE PROC proc_nhanvien
+@ten NVARCHAR(100),
+AS
+BEGIN
+SELECT * FROM func_nhanvien(@ten)
+END
+GO
+exec proc_nhanvien 'hiendam'</t>
+  </si>
+  <si>
+    <t>BÀI TẬP SQL DAY 1</t>
+  </si>
+  <si>
+    <t>BÀI TẬP SQL DAY 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +178,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -148,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -180,12 +232,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -207,6 +319,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -525,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D738DB1-E49F-4F9C-BC80-259031F7F0D1}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,7 +666,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -656,4 +783,79 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1216B59D-FD6A-44C3-B444-F247062FF276}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="11"/>
+    <col min="2" max="2" width="51.5546875" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="145.80000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>